<commit_message>
Registro de pago de alumno con id de profesor.
Se implementa (o corrige) el caso de uso registrar pago de alumno, se guarda un profesor con un id y se muestre solo los pagos registrados en un grupo a un profesor.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 6ta Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 6ta Iteración.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19226"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\UV - Ingeniería de Software\6to Semestre\Desarrollo de Software\1er Parcial\Tareas y Trabajos\Clon Repo\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55A09E30-3AB7-4DDD-A7C3-F121C26763A7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7FC0524B-BAF7-40C6-8C4C-DAE7989F74A0}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="52">
   <si>
     <t>Columna</t>
   </si>
@@ -184,6 +184,9 @@
   </si>
   <si>
     <t>Victor</t>
+  </si>
+  <si>
+    <t>Hecho</t>
   </si>
 </sst>
 </file>
@@ -396,12 +399,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -412,6 +409,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -724,7 +727,7 @@
       <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="N9" sqref="N9"/>
+      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -799,84 +802,84 @@
       </c>
     </row>
     <row r="4" spans="2:53" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H4" s="15" t="s">
+      <c r="H4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="16"/>
+      <c r="I4" s="20"/>
       <c r="J4" s="9"/>
-      <c r="K4" s="15" t="s">
+      <c r="K4" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="16"/>
+      <c r="L4" s="20"/>
       <c r="M4" s="9"/>
-      <c r="N4" s="15" t="s">
+      <c r="N4" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="O4" s="16"/>
+      <c r="O4" s="20"/>
       <c r="P4" s="9"/>
-      <c r="Q4" s="15" t="s">
+      <c r="Q4" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="R4" s="16"/>
+      <c r="R4" s="20"/>
       <c r="S4" s="9"/>
-      <c r="T4" s="15" t="s">
+      <c r="T4" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="U4" s="16"/>
+      <c r="U4" s="20"/>
       <c r="V4" s="9"/>
-      <c r="W4" s="15" t="s">
+      <c r="W4" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="X4" s="16"/>
+      <c r="X4" s="20"/>
       <c r="Y4" s="9"/>
-      <c r="Z4" s="15" t="s">
+      <c r="Z4" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="AA4" s="16"/>
+      <c r="AA4" s="20"/>
       <c r="AB4" s="9"/>
-      <c r="AC4" s="15" t="s">
+      <c r="AC4" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="AD4" s="16"/>
+      <c r="AD4" s="20"/>
       <c r="AE4" s="9"/>
-      <c r="AF4" s="15" t="s">
+      <c r="AF4" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="AG4" s="16"/>
+      <c r="AG4" s="20"/>
       <c r="AH4" s="9"/>
-      <c r="AI4" s="15" t="s">
+      <c r="AI4" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="AJ4" s="16"/>
+      <c r="AJ4" s="20"/>
       <c r="AK4" s="9"/>
-      <c r="AL4" s="15" t="s">
+      <c r="AL4" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="AM4" s="16"/>
+      <c r="AM4" s="20"/>
       <c r="AN4" s="9"/>
-      <c r="AO4" s="15" t="s">
+      <c r="AO4" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="AP4" s="16"/>
+      <c r="AP4" s="20"/>
       <c r="AQ4" s="9"/>
-      <c r="AR4" s="15" t="s">
+      <c r="AR4" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="AS4" s="16"/>
+      <c r="AS4" s="20"/>
       <c r="AT4" s="9"/>
-      <c r="AU4" s="15" t="s">
+      <c r="AU4" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="AV4" s="16"/>
+      <c r="AV4" s="20"/>
       <c r="AW4" s="9"/>
-      <c r="AX4" s="15" t="s">
+      <c r="AX4" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="AY4" s="16"/>
-      <c r="AZ4" s="15" t="s">
+      <c r="AY4" s="20"/>
+      <c r="AZ4" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="BA4" s="16"/>
+      <c r="BA4" s="20"/>
     </row>
     <row r="5" spans="2:53" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
@@ -1011,10 +1014,10 @@
     <row r="6" spans="2:53" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="17" t="s">
         <v>50</v>
       </c>
       <c r="F6" s="5" t="s">
@@ -1124,10 +1127,10 @@
     <row r="7" spans="2:53" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="18" t="s">
         <v>40</v>
       </c>
       <c r="F7" s="5" t="s">
@@ -1237,10 +1240,10 @@
     <row r="8" spans="2:53" x14ac:dyDescent="0.25">
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="17" t="s">
         <v>50</v>
       </c>
       <c r="F8" s="5" t="s">
@@ -1350,10 +1353,10 @@
     <row r="9" spans="2:53" ht="75" x14ac:dyDescent="0.25">
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="E9" s="20" t="s">
+      <c r="E9" s="18" t="s">
         <v>40</v>
       </c>
       <c r="F9" s="5" t="s">
@@ -1463,10 +1466,10 @@
     <row r="10" spans="2:53" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="E10" s="17" t="s">
         <v>50</v>
       </c>
       <c r="F10" s="5" t="s">
@@ -1579,120 +1582,122 @@
       <c r="D11" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="E11" s="18" t="s">
         <v>40</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="G11" s="5">
         <v>4</v>
       </c>
-      <c r="H11" s="8"/>
+      <c r="H11" s="8">
+        <v>3</v>
+      </c>
       <c r="I11" s="8">
         <f>G11-H11</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J11" s="10"/>
       <c r="K11" s="8"/>
       <c r="L11" s="8">
         <f>I11-K11</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M11" s="10"/>
       <c r="N11" s="8"/>
       <c r="O11" s="8">
         <f>L11-N11</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="P11" s="10"/>
       <c r="Q11" s="8"/>
       <c r="R11" s="8">
         <f>O11-Q11</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="S11" s="10"/>
       <c r="T11" s="8"/>
       <c r="U11" s="8">
         <f>R11-T11</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="V11" s="10"/>
       <c r="W11" s="8"/>
       <c r="X11" s="8">
         <f>U11-W11</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="Y11" s="10"/>
       <c r="Z11" s="8"/>
       <c r="AA11" s="8">
         <f>X11-Z11</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AB11" s="10"/>
       <c r="AC11" s="8"/>
       <c r="AD11" s="8">
         <f>AA11-AC11</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AE11" s="10"/>
       <c r="AF11" s="8"/>
       <c r="AG11" s="8">
         <f>AD11-AF11</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AH11" s="10"/>
       <c r="AI11" s="8"/>
       <c r="AJ11" s="8">
         <f>AG11-AI11</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AK11" s="10"/>
       <c r="AL11" s="8"/>
       <c r="AM11" s="8">
         <f>AJ11-AL11</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AN11" s="10"/>
       <c r="AO11" s="8"/>
       <c r="AP11" s="8">
         <f>AM11-AO11</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AQ11" s="10"/>
       <c r="AR11" s="8"/>
       <c r="AS11" s="8">
         <f>AP11-AR11</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AT11" s="10"/>
       <c r="AU11" s="8"/>
       <c r="AV11" s="8">
         <f>AS11-AU11</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AW11" s="10"/>
       <c r="AX11" s="8"/>
       <c r="AY11" s="8">
         <f>AV11-AX11</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AZ11" s="11">
         <f>H11+K11+N11+Q11+T11+W11+Z11+AC11+AF11+AI11+AL11+AO11+AR11+AU11+AX11</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BA11" s="11">
         <f>G11-AZ11</f>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:53" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="E12" s="19" t="s">
+      <c r="E12" s="17" t="s">
         <v>50</v>
       </c>
       <c r="F12" s="5" t="s">
@@ -1802,10 +1807,10 @@
     <row r="13" spans="2:53" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="E13" s="18" t="s">
         <v>40</v>
       </c>
       <c r="F13" s="5" t="s">
@@ -1915,7 +1920,7 @@
     <row r="14" spans="2:53" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
-      <c r="D14" s="18"/>
+      <c r="D14" s="16"/>
       <c r="E14" s="14"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
@@ -2020,7 +2025,7 @@
     <row r="15" spans="2:53" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
-      <c r="D15" s="17"/>
+      <c r="D15" s="15"/>
       <c r="E15" s="14"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
@@ -2543,11 +2548,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2559,6 +2559,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
CRU Renta de espacio
Se implementa la renta de espacio, faltando unicamente los datos
correspondientes al pago y se actualizan plantillas de CU y lista de
tareas.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 6ta Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 6ta Iteración.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7FC0524B-BAF7-40C6-8C4C-DAE7989F74A0}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E85CDE71-374F-402A-AFFA-BCC05AC2737B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="53">
   <si>
     <t>Columna</t>
   </si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t>Hecho</t>
+  </si>
+  <si>
+    <t>En proceso</t>
   </si>
 </sst>
 </file>
@@ -727,7 +730,7 @@
       <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomRight" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1247,107 +1250,109 @@
         <v>50</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="G8" s="5">
         <v>4</v>
       </c>
-      <c r="H8" s="8"/>
+      <c r="H8" s="8">
+        <v>3</v>
+      </c>
       <c r="I8" s="8">
         <f t="shared" si="16"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J8" s="10"/>
       <c r="K8" s="8"/>
       <c r="L8" s="8">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M8" s="10"/>
       <c r="N8" s="8"/>
       <c r="O8" s="8">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="P8" s="10"/>
       <c r="Q8" s="8"/>
       <c r="R8" s="8">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="S8" s="10"/>
       <c r="T8" s="8"/>
       <c r="U8" s="8">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="V8" s="10"/>
       <c r="W8" s="8"/>
       <c r="X8" s="8">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="Y8" s="10"/>
       <c r="Z8" s="8"/>
       <c r="AA8" s="8">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AB8" s="10"/>
       <c r="AC8" s="8"/>
       <c r="AD8" s="8">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AE8" s="10"/>
       <c r="AF8" s="8"/>
       <c r="AG8" s="8">
         <f t="shared" si="7"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AH8" s="10"/>
       <c r="AI8" s="8"/>
       <c r="AJ8" s="8">
         <f t="shared" si="8"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AK8" s="10"/>
       <c r="AL8" s="8"/>
       <c r="AM8" s="8">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AN8" s="10"/>
       <c r="AO8" s="8"/>
       <c r="AP8" s="8">
         <f t="shared" si="10"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AQ8" s="10"/>
       <c r="AR8" s="8"/>
       <c r="AS8" s="8">
         <f t="shared" si="11"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AT8" s="10"/>
       <c r="AU8" s="8"/>
       <c r="AV8" s="8">
         <f t="shared" si="12"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AW8" s="10"/>
       <c r="AX8" s="8"/>
       <c r="AY8" s="8">
         <f t="shared" si="13"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AZ8" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BA8" s="11">
         <f t="shared" si="15"/>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:53" ht="75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Implementacion del caso de uso obtener rentas cliente
Se implementa el caso de uso obtener rentas cliente, se actualizan las tablas de pruebas y la lista de tareas de la iteracion.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 6ta Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 6ta Iteración.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8829805E-6276-4019-B135-1EDE8BBF9B53}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{31147424-D2E1-4B0A-8087-5D523FD33112}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -730,7 +730,7 @@
       <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="K9" sqref="K9"/>
+      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1137,7 +1137,7 @@
         <v>40</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="G7" s="5">
         <v>2</v>
@@ -1148,96 +1148,98 @@
         <v>2</v>
       </c>
       <c r="J7" s="10"/>
-      <c r="K7" s="8"/>
+      <c r="K7" s="8">
+        <v>4</v>
+      </c>
       <c r="L7" s="8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="M7" s="10"/>
       <c r="N7" s="8"/>
       <c r="O7" s="8">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="P7" s="10"/>
       <c r="Q7" s="8"/>
       <c r="R7" s="8">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="S7" s="10"/>
       <c r="T7" s="8"/>
       <c r="U7" s="8">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="V7" s="10"/>
       <c r="W7" s="8"/>
       <c r="X7" s="8">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="Y7" s="10"/>
       <c r="Z7" s="8"/>
       <c r="AA7" s="8">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="AB7" s="10"/>
       <c r="AC7" s="8"/>
       <c r="AD7" s="8">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="AE7" s="10"/>
       <c r="AF7" s="8"/>
       <c r="AG7" s="8">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="AH7" s="10"/>
       <c r="AI7" s="8"/>
       <c r="AJ7" s="8">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="AK7" s="10"/>
       <c r="AL7" s="8"/>
       <c r="AM7" s="8">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="AN7" s="10"/>
       <c r="AO7" s="8"/>
       <c r="AP7" s="8">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="AQ7" s="10"/>
       <c r="AR7" s="8"/>
       <c r="AS7" s="8">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="AT7" s="10"/>
       <c r="AU7" s="8"/>
       <c r="AV7" s="8">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="AW7" s="10"/>
       <c r="AX7" s="8"/>
       <c r="AY7" s="8">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="AZ7" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BA7" s="11">
         <f t="shared" si="15"/>
-        <v>2</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="8" spans="2:53" x14ac:dyDescent="0.25">
@@ -2555,11 +2557,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2571,6 +2568,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Panel clientes en la ventana principal
Se implementa el pago de los clientes en la ventana principal del director, se actualza la plantilla de la iteración
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 6ta Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 6ta Iteración.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE0160F-9397-4369-A231-E0A9510E786C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1303BAB4-432D-4106-99C0-2B9F17E2A753}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -730,7 +730,7 @@
       <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="N10" sqref="N10"/>
+      <selection pane="bottomRight" activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1158,90 +1158,92 @@
         <v>-2</v>
       </c>
       <c r="M7" s="10"/>
-      <c r="N7" s="8"/>
+      <c r="N7" s="8">
+        <v>1</v>
+      </c>
       <c r="O7" s="8">
         <f t="shared" si="1"/>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="P7" s="10"/>
       <c r="Q7" s="8"/>
       <c r="R7" s="8">
         <f t="shared" si="2"/>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="S7" s="10"/>
       <c r="T7" s="8"/>
       <c r="U7" s="8">
         <f t="shared" si="3"/>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="V7" s="10"/>
       <c r="W7" s="8"/>
       <c r="X7" s="8">
         <f t="shared" si="4"/>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="Y7" s="10"/>
       <c r="Z7" s="8"/>
       <c r="AA7" s="8">
         <f t="shared" si="5"/>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="AB7" s="10"/>
       <c r="AC7" s="8"/>
       <c r="AD7" s="8">
         <f t="shared" si="6"/>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="AE7" s="10"/>
       <c r="AF7" s="8"/>
       <c r="AG7" s="8">
         <f t="shared" si="7"/>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="AH7" s="10"/>
       <c r="AI7" s="8"/>
       <c r="AJ7" s="8">
         <f t="shared" si="8"/>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="AK7" s="10"/>
       <c r="AL7" s="8"/>
       <c r="AM7" s="8">
         <f t="shared" si="9"/>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="AN7" s="10"/>
       <c r="AO7" s="8"/>
       <c r="AP7" s="8">
         <f t="shared" si="10"/>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="AQ7" s="10"/>
       <c r="AR7" s="8"/>
       <c r="AS7" s="8">
         <f t="shared" si="11"/>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="AT7" s="10"/>
       <c r="AU7" s="8"/>
       <c r="AV7" s="8">
         <f t="shared" si="12"/>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="AW7" s="10"/>
       <c r="AX7" s="8"/>
       <c r="AY7" s="8">
         <f t="shared" si="13"/>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="AZ7" s="11">
         <f t="shared" si="14"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BA7" s="11">
         <f t="shared" si="15"/>
-        <v>-2</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="8" spans="2:53" x14ac:dyDescent="0.25">
@@ -2559,11 +2561,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2575,6 +2572,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Preubas de CRU Renta de espacio.
Pruebas para el caso de uso CRU Renta de espacio, se carga el panel de
asistencia desde un grupo y se actualizan plantillas de casos de uso y
tareas.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 6ta Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 6ta Iteración.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1303BAB4-432D-4106-99C0-2B9F17E2A753}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{513681C3-9D6A-4754-8F0D-B20DD0653890}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -730,7 +730,7 @@
       <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="N7" sqref="N7"/>
+      <selection pane="bottomRight" activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1024,7 +1024,7 @@
         <v>50</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="G6" s="5">
         <v>5</v>
@@ -1043,90 +1043,92 @@
         <v>4</v>
       </c>
       <c r="M6" s="10"/>
-      <c r="N6" s="8"/>
+      <c r="N6" s="8">
+        <v>1</v>
+      </c>
       <c r="O6" s="8">
         <f t="shared" ref="O6:O16" si="1">L6-N6</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P6" s="10"/>
       <c r="Q6" s="8"/>
       <c r="R6" s="8">
         <f t="shared" ref="R6:R16" si="2">O6-Q6</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S6" s="10"/>
       <c r="T6" s="8"/>
       <c r="U6" s="8">
         <f t="shared" ref="U6:U16" si="3">R6-T6</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V6" s="10"/>
       <c r="W6" s="8"/>
       <c r="X6" s="8">
         <f t="shared" ref="X6:X16" si="4">U6-W6</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y6" s="10"/>
       <c r="Z6" s="8"/>
       <c r="AA6" s="8">
         <f t="shared" ref="AA6:AA16" si="5">X6-Z6</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AB6" s="10"/>
       <c r="AC6" s="8"/>
       <c r="AD6" s="8">
         <f t="shared" ref="AD6:AD16" si="6">AA6-AC6</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE6" s="10"/>
       <c r="AF6" s="8"/>
       <c r="AG6" s="8">
         <f t="shared" ref="AG6:AG16" si="7">AD6-AF6</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AH6" s="10"/>
       <c r="AI6" s="8"/>
       <c r="AJ6" s="8">
         <f t="shared" ref="AJ6:AJ16" si="8">AG6-AI6</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AK6" s="10"/>
       <c r="AL6" s="8"/>
       <c r="AM6" s="8">
         <f t="shared" ref="AM6:AM16" si="9">AJ6-AL6</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AN6" s="10"/>
       <c r="AO6" s="8"/>
       <c r="AP6" s="8">
         <f t="shared" ref="AP6:AP16" si="10">AM6-AO6</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AQ6" s="10"/>
       <c r="AR6" s="8"/>
       <c r="AS6" s="8">
         <f t="shared" ref="AS6:AS16" si="11">AP6-AR6</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AT6" s="10"/>
       <c r="AU6" s="8"/>
       <c r="AV6" s="8">
         <f t="shared" ref="AV6:AV16" si="12">AS6-AU6</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AW6" s="10"/>
       <c r="AX6" s="8"/>
       <c r="AY6" s="8">
         <f t="shared" ref="AY6:AY16" si="13">AV6-AX6</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AZ6" s="11">
         <f t="shared" ref="AZ6:AZ16" si="14">H6+K6+N6+Q6+T6+W6+Z6+AC6+AF6+AI6+AL6+AO6+AR6+AU6+AX6</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BA6" s="11">
         <f t="shared" ref="BA6:BA16" si="15">G6-AZ6</f>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="2:53" ht="30" x14ac:dyDescent="0.25">
@@ -1256,7 +1258,7 @@
         <v>50</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G8" s="5">
         <v>4</v>
@@ -1277,90 +1279,92 @@
         <v>0</v>
       </c>
       <c r="M8" s="10"/>
-      <c r="N8" s="8"/>
+      <c r="N8" s="8">
+        <v>1</v>
+      </c>
       <c r="O8" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="P8" s="10"/>
       <c r="Q8" s="8"/>
       <c r="R8" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="S8" s="10"/>
       <c r="T8" s="8"/>
       <c r="U8" s="8">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="V8" s="10"/>
       <c r="W8" s="8"/>
       <c r="X8" s="8">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y8" s="10"/>
       <c r="Z8" s="8"/>
       <c r="AA8" s="8">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AB8" s="10"/>
       <c r="AC8" s="8"/>
       <c r="AD8" s="8">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AE8" s="10"/>
       <c r="AF8" s="8"/>
       <c r="AG8" s="8">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AH8" s="10"/>
       <c r="AI8" s="8"/>
       <c r="AJ8" s="8">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AK8" s="10"/>
       <c r="AL8" s="8"/>
       <c r="AM8" s="8">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AN8" s="10"/>
       <c r="AO8" s="8"/>
       <c r="AP8" s="8">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AQ8" s="10"/>
       <c r="AR8" s="8"/>
       <c r="AS8" s="8">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AT8" s="10"/>
       <c r="AU8" s="8"/>
       <c r="AV8" s="8">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AW8" s="10"/>
       <c r="AX8" s="8"/>
       <c r="AY8" s="8">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AZ8" s="11">
         <f t="shared" si="14"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BA8" s="11">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="9" spans="2:53" ht="75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Corrección de textos y caso de uso cambiar alumno de grupo.
Se corrigen los textos del proyecto asi como se modifico la muestra de grupos en el caso de uso cambiar alumno de grupo
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 6ta Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 6ta Iteración.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{513681C3-9D6A-4754-8F0D-B20DD0653890}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{18AF0320-6195-4422-BC54-DFBE38284203}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -730,7 +730,7 @@
       <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="O10" sqref="O10"/>
+      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1377,107 +1377,109 @@
         <v>40</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="G9" s="5">
         <v>2</v>
       </c>
-      <c r="H9" s="8"/>
+      <c r="H9" s="8">
+        <v>2</v>
+      </c>
       <c r="I9" s="8">
         <f t="shared" si="16"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J9" s="10"/>
       <c r="K9" s="8"/>
       <c r="L9" s="8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M9" s="10"/>
       <c r="N9" s="8"/>
       <c r="O9" s="8">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P9" s="10"/>
       <c r="Q9" s="8"/>
       <c r="R9" s="8">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S9" s="10"/>
       <c r="T9" s="8"/>
       <c r="U9" s="8">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V9" s="10"/>
       <c r="W9" s="8"/>
       <c r="X9" s="8">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Y9" s="10"/>
       <c r="Z9" s="8"/>
       <c r="AA9" s="8">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB9" s="10"/>
       <c r="AC9" s="8"/>
       <c r="AD9" s="8">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AE9" s="10"/>
       <c r="AF9" s="8"/>
       <c r="AG9" s="8">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AH9" s="10"/>
       <c r="AI9" s="8"/>
       <c r="AJ9" s="8">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AK9" s="10"/>
       <c r="AL9" s="8"/>
       <c r="AM9" s="8">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AN9" s="10"/>
       <c r="AO9" s="8"/>
       <c r="AP9" s="8">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AQ9" s="10"/>
       <c r="AR9" s="8"/>
       <c r="AS9" s="8">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AT9" s="10"/>
       <c r="AU9" s="8"/>
       <c r="AV9" s="8">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AW9" s="10"/>
       <c r="AX9" s="8"/>
       <c r="AY9" s="8">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AZ9" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA9" s="11">
         <f t="shared" si="15"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:53" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2565,6 +2567,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2576,11 +2583,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Margenés de la interfaz gráfica
Se validan los márgenes de todas las interfaces gráficas y se actualiza
plantilla de tareas de la iteración.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 6ta Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 6ta Iteración.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\UV - Ingeniería de Software\6to Semestre\Desarrollo de Software\1er Parcial\Tareas y Trabajos\Clon Repo\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF40086B-566B-4735-9B31-868D713BA09A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A6DD075-5E5B-4794-915A-34DD875FF8AB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="52">
   <si>
     <t>Columna</t>
   </si>
@@ -187,9 +187,6 @@
   </si>
   <si>
     <t>Hecho</t>
-  </si>
-  <si>
-    <t>En proceso</t>
   </si>
 </sst>
 </file>
@@ -730,7 +727,7 @@
       <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="O10" sqref="O10"/>
+      <selection pane="bottomRight" activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1024,7 +1021,7 @@
         <v>50</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G6" s="5">
         <v>5</v>
@@ -1494,7 +1491,7 @@
         <v>50</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="G10" s="5">
         <v>2</v>
@@ -1523,78 +1520,80 @@
         <v>4</v>
       </c>
       <c r="S10" s="10"/>
-      <c r="T10" s="8"/>
+      <c r="T10" s="8">
+        <v>2</v>
+      </c>
       <c r="U10" s="8">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="V10" s="10"/>
       <c r="W10" s="8"/>
       <c r="X10" s="8">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Y10" s="10"/>
       <c r="Z10" s="8"/>
       <c r="AA10" s="8">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AB10" s="10"/>
       <c r="AC10" s="8"/>
       <c r="AD10" s="8">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AE10" s="10"/>
       <c r="AF10" s="8"/>
       <c r="AG10" s="8">
         <f t="shared" si="7"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AH10" s="10"/>
       <c r="AI10" s="8"/>
       <c r="AJ10" s="8">
         <f t="shared" si="8"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AK10" s="10"/>
       <c r="AL10" s="8"/>
       <c r="AM10" s="8">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AN10" s="10"/>
       <c r="AO10" s="8"/>
       <c r="AP10" s="8">
         <f t="shared" si="10"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AQ10" s="10"/>
       <c r="AR10" s="8"/>
       <c r="AS10" s="8">
         <f t="shared" si="11"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AT10" s="10"/>
       <c r="AU10" s="8"/>
       <c r="AV10" s="8">
         <f t="shared" si="12"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AW10" s="10"/>
       <c r="AX10" s="8"/>
       <c r="AY10" s="8">
         <f t="shared" si="13"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AZ10" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA10" s="11">
         <f t="shared" si="15"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:53" ht="96" customHeight="1" x14ac:dyDescent="0.25">
@@ -2569,6 +2568,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2580,11 +2584,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Se modifica y valida la implementacion del caso de uso registrar pago alumno
Se corrige la seleccion de promociones en el caso de uso registrar pago de alumno
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 6ta Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 6ta Iteración.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\UV - Ingeniería de Software\6to Semestre\Desarrollo de Software\1er Parcial\Tareas y Trabajos\Clon Repo\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A6DD075-5E5B-4794-915A-34DD875FF8AB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1443DB8C-AA5E-44DF-9D96-E43A9DC94880}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="53">
   <si>
     <t>Columna</t>
   </si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t>Hecho</t>
+  </si>
+  <si>
+    <t>Validar que se cierra la ventana de selección de promociones despes de elegida una.</t>
   </si>
 </sst>
 </file>
@@ -727,7 +730,7 @@
       <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="K9" sqref="K9"/>
+      <selection pane="bottomRight" activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1940,41 +1943,51 @@
     <row r="14" spans="2:53" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
+      <c r="D14" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G14" s="5">
+        <v>2</v>
+      </c>
       <c r="H14" s="8"/>
       <c r="I14" s="8">
         <f>G14-H14</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J14" s="10"/>
       <c r="K14" s="8"/>
       <c r="L14" s="8">
         <f>I14-K14</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M14" s="10"/>
       <c r="N14" s="8"/>
       <c r="O14" s="8">
         <f>L14-N14</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P14" s="10"/>
       <c r="Q14" s="8"/>
       <c r="R14" s="8">
         <f>O14-Q14</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S14" s="10"/>
       <c r="T14" s="8"/>
       <c r="U14" s="8">
         <f>R14-T14</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V14" s="10"/>
-      <c r="W14" s="8"/>
+      <c r="W14" s="8">
+        <v>2</v>
+      </c>
       <c r="X14" s="8">
         <f>U14-W14</f>
         <v>0</v>
@@ -2035,7 +2048,7 @@
       </c>
       <c r="AZ14" s="11">
         <f>H14+K14+N14+Q14+T14+W14+Z14+AC14+AF14+AI14+AL14+AO14+AR14+AU14+AX14</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA14" s="11">
         <f>G14-AZ14</f>
@@ -2568,11 +2581,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2584,6 +2592,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Diagrama de clases actualizado
Se actualiza diagrama de clases y la plantilla de lista de tareas de la
iteración.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 6ta Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 6ta Iteración.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1443DB8C-AA5E-44DF-9D96-E43A9DC94880}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9884E019-FC2F-46D9-83F6-318E18C0B47A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="52">
   <si>
     <t>Columna</t>
   </si>
@@ -187,9 +187,6 @@
   </si>
   <si>
     <t>Hecho</t>
-  </si>
-  <si>
-    <t>Validar que se cierra la ventana de selección de promociones despes de elegida una.</t>
   </si>
 </sst>
 </file>
@@ -727,10 +724,10 @@
   <dimension ref="B1:BA19"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="G9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="G13" sqref="G13"/>
+      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1724,7 +1721,7 @@
         <v>50</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="G12" s="5">
         <v>2</v>
@@ -1759,72 +1756,74 @@
         <v>2</v>
       </c>
       <c r="V12" s="10"/>
-      <c r="W12" s="8"/>
+      <c r="W12" s="8">
+        <v>2</v>
+      </c>
       <c r="X12" s="8">
         <f>U12-W12</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Y12" s="10"/>
       <c r="Z12" s="8"/>
       <c r="AA12" s="8">
         <f>X12-Z12</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB12" s="10"/>
       <c r="AC12" s="8"/>
       <c r="AD12" s="8">
         <f>AA12-AC12</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AE12" s="10"/>
       <c r="AF12" s="8"/>
       <c r="AG12" s="8">
         <f>AD12-AF12</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AH12" s="10"/>
       <c r="AI12" s="8"/>
       <c r="AJ12" s="8">
         <f>AG12-AI12</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AK12" s="10"/>
       <c r="AL12" s="8"/>
       <c r="AM12" s="8">
         <f>AJ12-AL12</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AN12" s="10"/>
       <c r="AO12" s="8"/>
       <c r="AP12" s="8">
         <f>AM12-AO12</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AQ12" s="10"/>
       <c r="AR12" s="8"/>
       <c r="AS12" s="8">
         <f>AP12-AR12</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AT12" s="10"/>
       <c r="AU12" s="8"/>
       <c r="AV12" s="8">
         <f>AS12-AU12</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AW12" s="10"/>
       <c r="AX12" s="8"/>
       <c r="AY12" s="8">
         <f>AV12-AX12</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AZ12" s="11">
         <f>H12+K12+N12+Q12+T12+W12+Z12+AC12+AF12+AI12+AL12+AO12+AR12+AU12+AX12</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA12" s="11">
         <f>G12-AZ12</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:53" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1943,51 +1942,41 @@
     <row r="14" spans="2:53" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
-      <c r="D14" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="E14" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G14" s="5">
-        <v>2</v>
-      </c>
+      <c r="D14" s="16"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
       <c r="H14" s="8"/>
       <c r="I14" s="8">
         <f>G14-H14</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J14" s="10"/>
       <c r="K14" s="8"/>
       <c r="L14" s="8">
         <f>I14-K14</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M14" s="10"/>
       <c r="N14" s="8"/>
       <c r="O14" s="8">
         <f>L14-N14</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P14" s="10"/>
       <c r="Q14" s="8"/>
       <c r="R14" s="8">
         <f>O14-Q14</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S14" s="10"/>
       <c r="T14" s="8"/>
       <c r="U14" s="8">
         <f>R14-T14</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V14" s="10"/>
-      <c r="W14" s="8">
-        <v>2</v>
-      </c>
+      <c r="W14" s="8"/>
       <c r="X14" s="8">
         <f>U14-W14</f>
         <v>0</v>
@@ -2048,7 +2037,7 @@
       </c>
       <c r="AZ14" s="11">
         <f>H14+K14+N14+Q14+T14+W14+Z14+AC14+AF14+AI14+AL14+AO14+AR14+AU14+AX14</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BA14" s="11">
         <f>G14-AZ14</f>
@@ -2581,6 +2570,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2592,11 +2586,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualización del diagrama de paquetes.
Se actualiza el diagrama de paquetes y correcciones en el caso de uso registrar pago alumno
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 6ta Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 6ta Iteración.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9884E019-FC2F-46D9-83F6-318E18C0B47A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{92073B2D-D174-4617-8462-6CFE3A63CCE4}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="51">
   <si>
     <t>Columna</t>
   </si>
@@ -154,9 +154,6 @@
   </si>
   <si>
     <t>Mario</t>
-  </si>
-  <si>
-    <t>Por iniciar</t>
   </si>
   <si>
     <t>CU - Registrar asistencia</t>
@@ -724,10 +721,10 @@
   <dimension ref="B1:BA19"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="G9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomRight" activeCell="W13" sqref="W13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1015,13 +1012,13 @@
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E6" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>51</v>
       </c>
       <c r="G6" s="5">
         <v>5</v>
@@ -1134,13 +1131,13 @@
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E7" s="18" t="s">
         <v>40</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G7" s="5">
         <v>2</v>
@@ -1251,13 +1248,13 @@
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="F8" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>51</v>
       </c>
       <c r="G8" s="5">
         <v>4</v>
@@ -1370,13 +1367,13 @@
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E9" s="18" t="s">
         <v>40</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G9" s="5">
         <v>2</v>
@@ -1485,13 +1482,13 @@
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E10" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>51</v>
       </c>
       <c r="G10" s="5">
         <v>2</v>
@@ -1600,13 +1597,13 @@
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E11" s="18" t="s">
         <v>40</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G11" s="5">
         <v>4</v>
@@ -1715,13 +1712,13 @@
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E12" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>51</v>
       </c>
       <c r="G12" s="5">
         <v>2</v>
@@ -1830,13 +1827,13 @@
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E13" s="18" t="s">
         <v>40</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="G13" s="5">
         <v>1</v>
@@ -1871,72 +1868,74 @@
         <v>1</v>
       </c>
       <c r="V13" s="10"/>
-      <c r="W13" s="8"/>
+      <c r="W13" s="8">
+        <v>1</v>
+      </c>
       <c r="X13" s="8">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y13" s="10"/>
       <c r="Z13" s="8"/>
       <c r="AA13" s="8">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB13" s="10"/>
       <c r="AC13" s="8"/>
       <c r="AD13" s="8">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE13" s="10"/>
       <c r="AF13" s="8"/>
       <c r="AG13" s="8">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH13" s="10"/>
       <c r="AI13" s="8"/>
       <c r="AJ13" s="8">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK13" s="10"/>
       <c r="AL13" s="8"/>
       <c r="AM13" s="8">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN13" s="10"/>
       <c r="AO13" s="8"/>
       <c r="AP13" s="8">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ13" s="10"/>
       <c r="AR13" s="8"/>
       <c r="AS13" s="8">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT13" s="10"/>
       <c r="AU13" s="8"/>
       <c r="AV13" s="8">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW13" s="10"/>
       <c r="AX13" s="8"/>
       <c r="AY13" s="8">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ13" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA13" s="11">
         <f t="shared" si="15"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:53" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2570,11 +2569,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2586,6 +2580,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>